<commit_message>
change to excel sheet
</commit_message>
<xml_diff>
--- a/hihi.xlsx
+++ b/hihi.xlsx
@@ -1,39 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26408"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TopherBarnett/Projects/excel-python/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>test</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,11 +52,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -121,12 +98,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -153,15 +130,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -188,7 +164,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -364,16 +339,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -384,7 +357,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>12</v>
       </c>
@@ -395,7 +368,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>23</v>
       </c>
@@ -406,7 +379,7 @@
         <v>103.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>34</v>
       </c>
@@ -417,7 +390,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>45</v>
       </c>
@@ -428,7 +401,7 @@
         <v>202.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>56</v>
       </c>
@@ -439,7 +412,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>67</v>
       </c>
@@ -450,18 +423,18 @@
         <v>301.5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>78</v>
       </c>
-      <c r="B8" t="s">
-        <v>0</v>
+      <c r="B8">
+        <v>234</v>
       </c>
       <c r="C8">
         <v>351</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>89</v>
       </c>
@@ -472,7 +445,7 @@
         <v>400.5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>100</v>
       </c>
@@ -483,7 +456,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>111</v>
       </c>
@@ -494,7 +467,7 @@
         <v>499.5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>122</v>
       </c>
@@ -505,7 +478,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>133</v>
       </c>
@@ -516,7 +489,7 @@
         <v>598.5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>144</v>
       </c>
@@ -527,7 +500,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>155</v>
       </c>
@@ -538,7 +511,7 @@
         <v>697.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>166</v>
       </c>
@@ -549,7 +522,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>177</v>
       </c>
@@ -560,7 +533,7 @@
         <v>796.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>188</v>
       </c>
@@ -571,7 +544,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>199</v>
       </c>
@@ -582,7 +555,7 @@
         <v>895.5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>210</v>
       </c>
@@ -593,7 +566,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>221</v>
       </c>
@@ -604,7 +577,7 @@
         <v>994.5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>232</v>
       </c>
@@ -615,7 +588,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>243</v>
       </c>
@@ -626,7 +599,7 @@
         <v>1093.5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>254</v>
       </c>
@@ -637,7 +610,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>265</v>
       </c>
@@ -648,7 +621,7 @@
         <v>1192.5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>276</v>
       </c>
@@ -659,7 +632,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>287</v>
       </c>
@@ -670,7 +643,7 @@
         <v>1291.5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>298</v>
       </c>
@@ -681,7 +654,7 @@
         <v>1341</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>309</v>
       </c>
@@ -692,7 +665,7 @@
         <v>1390.5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>320</v>
       </c>
@@ -703,7 +676,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>331</v>
       </c>
@@ -714,7 +687,7 @@
         <v>1489.5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>342</v>
       </c>
@@ -725,7 +698,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>353</v>
       </c>
@@ -736,7 +709,7 @@
         <v>1588.5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34">
         <v>364</v>
       </c>
@@ -747,7 +720,7 @@
         <v>1638</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="A35">
         <v>375</v>
       </c>
@@ -758,7 +731,7 @@
         <v>1687.5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>386</v>
       </c>
@@ -769,7 +742,7 @@
         <v>1737</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>397</v>
       </c>
@@ -780,7 +753,7 @@
         <v>1786.5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>408</v>
       </c>
@@ -791,7 +764,7 @@
         <v>1836</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>419</v>
       </c>
@@ -802,7 +775,7 @@
         <v>1885.5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>430</v>
       </c>
@@ -813,7 +786,7 @@
         <v>1935</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>441</v>
       </c>
@@ -824,7 +797,7 @@
         <v>1984.5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3">
       <c r="A42">
         <v>452</v>
       </c>
@@ -835,7 +808,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3">
       <c r="A43">
         <v>463</v>
       </c>
@@ -846,7 +819,7 @@
         <v>2083.5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3">
       <c r="A44">
         <v>474</v>
       </c>
@@ -857,7 +830,7 @@
         <v>2133</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3">
       <c r="A45">
         <v>485</v>
       </c>
@@ -868,7 +841,7 @@
         <v>2182.5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3">
       <c r="A46">
         <v>496</v>
       </c>
@@ -879,7 +852,7 @@
         <v>2232</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3">
       <c r="A47">
         <v>507</v>
       </c>
@@ -890,7 +863,7 @@
         <v>2281.5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3">
       <c r="A48">
         <v>518</v>
       </c>
@@ -901,7 +874,7 @@
         <v>2331</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3">
       <c r="A49">
         <v>529</v>
       </c>
@@ -912,7 +885,7 @@
         <v>2380.5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3">
       <c r="A50">
         <v>540</v>
       </c>
@@ -923,7 +896,7 @@
         <v>2430</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3">
       <c r="A51">
         <v>551</v>
       </c>
@@ -934,7 +907,7 @@
         <v>2479.5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3">
       <c r="A52">
         <v>562</v>
       </c>
@@ -945,7 +918,7 @@
         <v>2529</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3">
       <c r="A53">
         <v>573</v>
       </c>
@@ -956,7 +929,7 @@
         <v>2578.5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3">
       <c r="A54">
         <v>584</v>
       </c>
@@ -967,7 +940,7 @@
         <v>2628</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3">
       <c r="A55">
         <v>595</v>
       </c>
@@ -978,7 +951,7 @@
         <v>2677.5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3">
       <c r="A56">
         <v>606</v>
       </c>
@@ -989,7 +962,7 @@
         <v>2727</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3">
       <c r="A57">
         <v>617</v>
       </c>
@@ -1000,7 +973,7 @@
         <v>2776.5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3">
       <c r="A58">
         <v>628</v>
       </c>
@@ -1011,7 +984,7 @@
         <v>2826</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3">
       <c r="A59">
         <v>639</v>
       </c>
@@ -1022,7 +995,7 @@
         <v>2875.5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3">
       <c r="A60">
         <v>650</v>
       </c>
@@ -1033,7 +1006,7 @@
         <v>2925</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3">
       <c r="A61">
         <v>661</v>
       </c>
@@ -1044,7 +1017,7 @@
         <v>2974.5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3">
       <c r="A62">
         <v>672</v>
       </c>
@@ -1055,7 +1028,7 @@
         <v>3024</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3">
       <c r="A63">
         <v>683</v>
       </c>
@@ -1066,7 +1039,7 @@
         <v>3073.5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3">
       <c r="A64">
         <v>694</v>
       </c>
@@ -1077,7 +1050,7 @@
         <v>3123</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3">
       <c r="A65">
         <v>705</v>
       </c>
@@ -1088,7 +1061,7 @@
         <v>3172.5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3">
       <c r="A66">
         <v>716</v>
       </c>
@@ -1099,7 +1072,7 @@
         <v>3222</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3">
       <c r="A67">
         <v>727</v>
       </c>
@@ -1110,7 +1083,7 @@
         <v>3271.5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3">
       <c r="A68">
         <v>738</v>
       </c>
@@ -1121,7 +1094,7 @@
         <v>3321</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3">
       <c r="A69">
         <v>749</v>
       </c>
@@ -1132,7 +1105,7 @@
         <v>3370.5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3">
       <c r="A70">
         <v>760</v>
       </c>
@@ -1143,7 +1116,7 @@
         <v>3420</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3">
       <c r="A71">
         <v>771</v>
       </c>
@@ -1154,7 +1127,7 @@
         <v>3469.5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3">
       <c r="A72">
         <v>782</v>
       </c>
@@ -1165,7 +1138,7 @@
         <v>3519</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3">
       <c r="A73">
         <v>793</v>
       </c>
@@ -1176,7 +1149,7 @@
         <v>3568.5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3">
       <c r="A74">
         <v>804</v>
       </c>
@@ -1187,7 +1160,7 @@
         <v>3618</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3">
       <c r="A75">
         <v>815</v>
       </c>
@@ -1198,7 +1171,7 @@
         <v>3667.5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3">
       <c r="A76">
         <v>826</v>
       </c>
@@ -1209,7 +1182,7 @@
         <v>3717</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3">
       <c r="A77">
         <v>837</v>
       </c>
@@ -1220,7 +1193,7 @@
         <v>3766.5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3">
       <c r="A78">
         <v>848</v>
       </c>
@@ -1231,7 +1204,7 @@
         <v>3816</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3">
       <c r="A79">
         <v>859</v>
       </c>
@@ -1242,7 +1215,7 @@
         <v>3865.5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3">
       <c r="A80">
         <v>870</v>
       </c>
@@ -1253,7 +1226,7 @@
         <v>3915</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3">
       <c r="A81">
         <v>881</v>
       </c>
@@ -1264,7 +1237,7 @@
         <v>3964.5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3">
       <c r="A82">
         <v>892</v>
       </c>
@@ -1275,7 +1248,7 @@
         <v>4014</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3">
       <c r="A83">
         <v>903</v>
       </c>
@@ -1286,7 +1259,7 @@
         <v>4063.5</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3">
       <c r="A84">
         <v>914</v>
       </c>
@@ -1297,7 +1270,7 @@
         <v>4113</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3">
       <c r="A85">
         <v>925</v>
       </c>
@@ -1308,7 +1281,7 @@
         <v>4162.5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3">
       <c r="A86">
         <v>936</v>
       </c>
@@ -1319,7 +1292,7 @@
         <v>4212</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3">
       <c r="A87">
         <v>947</v>
       </c>
@@ -1330,7 +1303,7 @@
         <v>4261.5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3">
       <c r="A88">
         <v>958</v>
       </c>
@@ -1341,7 +1314,7 @@
         <v>4311</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3">
       <c r="A89">
         <v>969</v>
       </c>
@@ -1352,7 +1325,7 @@
         <v>4360.5</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3">
       <c r="A90">
         <v>980</v>
       </c>
@@ -1363,7 +1336,7 @@
         <v>4410</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3">
       <c r="A91">
         <v>991</v>
       </c>

</xml_diff>